<commit_message>
Fixed Excel Sheet for missing data
</commit_message>
<xml_diff>
--- a/seleniumgenc/src/test/java/excelFiles/ShopifyTestData.xlsx
+++ b/seleniumgenc/src/test/java/excelFiles/ShopifyTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\900466\eclipse-workspace\seleniumgenc\src\test\java\excelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\900466\git\Pipeline-Test\seleniumgenc\src\test\java\excelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719090FA-2DE8-47CF-8E79-396B088E3104}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924D1F85-0D81-491A-B9A9-A94964C916FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2050" yWindow="810" windowWidth="14400" windowHeight="7360" xr2:uid="{801A50C8-5D9E-4526-849F-9135B7E591E0}"/>
+    <workbookView xWindow="2050" yWindow="810" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{801A50C8-5D9E-4526-849F-9135B7E591E0}"/>
   </bookViews>
   <sheets>
     <sheet name="allFields" sheetId="1" r:id="rId1"/>
@@ -118,13 +118,17 @@
     <t>Lastname can't be blank</t>
   </si>
   <si>
-    <t>Firstname can't be blank\nLastname can't be blank\nUserName can't be blank\nPasswd can't be blank</t>
-  </si>
-  <si>
-    <t>Lastname can't be blank\nUserName can't be blank</t>
-  </si>
-  <si>
     <t>Jason Monroe JMoney Chennai</t>
+  </si>
+  <si>
+    <t>Lastname can't be blank
+UserName can't be blank</t>
+  </si>
+  <si>
+    <t>Firstname can't be blank
+Lastname can't be blank
+UserName can't be blank
+Passwd can't be blank</t>
   </si>
 </sst>
 </file>
@@ -160,8 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B398B3-95EC-408E-860D-90270A6FED2D}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -562,7 +569,7 @@
         <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -575,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401E9BB7-7F7E-4331-B003-93960F1BF350}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H7" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -687,7 +694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -700,19 +707,19 @@
       <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="174" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
       </c>
-      <c r="H7" t="s">
-        <v>27</v>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>